<commit_message>
try to fix lang son pipeline
</commit_message>
<xml_diff>
--- a/Scrape Logic/data_dat.xlsx
+++ b/Scrape Logic/data_dat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\estates-scraping-final\Scrape Logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2545842-19EA-4A49-9A50-B13EDDFA1CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912B46F5-64D4-4050-957A-8F778F40D07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,9 +238,6 @@
     </r>
   </si>
   <si>
-    <t>Trích xuất từ miêu tả trong bài đăng</t>
-  </si>
-  <si>
     <t>Nếu trích xuất được các cụm diện tích sàn, diện tích sử dụng thì sẽ lưu nó thành tổng diện tích sàn
 Nếu không có những cụm trên, tổng diện tích sàn sẽ được tính bằng diện tích xây dựng * tổng số tầng công trình. Diện tích xây dựng được xác định như sau:
 - Nếu có các cụm thổ cư / đất ở bao nhiêu m thì trả về giá trị xây dựng bằng giá trị được viết ở đây
@@ -329,10 +326,6 @@
     <t xml:space="preserve">Quy tắc </t>
   </si>
   <si>
-    <t xml:space="preserve">Nếu trong phần miêu tả hay tiêu đề có cụm "đất trồng" thì đất sẽ được phân vào loại hỗn hợp, còn không tất cả đều được quy về trường hợp đất ở
-</t>
-  </si>
-  <si>
     <t>Trích xuất từ miêu tả và tiêu đề trong bài đăng</t>
   </si>
   <si>
@@ -358,6 +351,20 @@
   </si>
   <si>
     <t>Chỉ lấy các trường hợp nhà cấp 4, nên đơn giá xây dựng sẽ là 4,000,000. Mặc định cho các khu đất vẫn là 0</t>
+  </si>
+  <si>
+    <t>Mục đích sử dụng đất sẽ được trích xuất theo các cụm sau:
+- Đất trồng lúa, đất trồng cây hằng năm, LUC, LUA, LUN, BHK,…: Đất trồng cây hằng năm
+- Đất trồng cây lâu năm, CLN, LNC, LNQ, LNK: Đất trồng cây lâu năm
+- Đất trồng cây, đất vườn: đất vườn
+- Đất rừng, RSX, RPH, RSN,...: Đất rừng
+- Đất nông nghiệp khác, NKH: Đất nông nghiệp khác
+- Đất ở, thổ cư, ONT, ODT: Đất ở
+- Đất khu công nghiệp, đất KCN, SKK,SKN, SKT: Đất khu công nghiệp
+- Đất thương mại, đất tm, tmdv, đất dịch vụ, đất dvu, đất kinh doanh: Đất thương mại, dịch vụ</t>
+  </si>
+  <si>
+    <t>Nếu khu đất có nhà thì sẽ trích xuất từ miêu tả trong bài đăng. Nếu không thì mặc định sẽ = 0</t>
   </si>
 </sst>
 </file>
@@ -403,12 +410,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -417,22 +439,22 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -717,406 +739,421 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="66.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="66.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D16" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="3" t="s">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="285" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>24</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="8" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="225" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="C31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>